<commit_message>
ubah sum pada excel
</commit_message>
<xml_diff>
--- a/docs/Kelompok5_DecisionTree_TugasAkhir.xlsx
+++ b/docs/Kelompok5_DecisionTree_TugasAkhir.xlsx
@@ -448,20 +448,36 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -490,22 +506,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2284,8 +2284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2315,44 +2315,44 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="30">
+      <c r="A2" s="17">
         <v>25</v>
       </c>
-      <c r="B2" s="30">
+      <c r="B2" s="17">
         <v>7.1</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="17" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="30">
+      <c r="A3" s="17">
         <v>27</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="18">
         <v>4.3</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="19" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="31">
+      <c r="A4" s="18">
         <v>20</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="18">
         <v>5</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -2365,16 +2365,16 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="30">
+      <c r="A5" s="17">
         <v>27</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="17">
         <v>7.2</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="2"/>
@@ -2385,16 +2385,16 @@
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="32">
+      <c r="A6" s="19">
         <v>30</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="17">
         <v>8</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="2"/>
@@ -2403,16 +2403,16 @@
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="30">
+      <c r="A7" s="17">
         <v>24</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="18">
         <v>5.4</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="19" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -2425,16 +2425,16 @@
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="30">
+      <c r="A8" s="17">
         <v>25</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="17">
         <v>6.7</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="2"/>
@@ -2445,16 +2445,16 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="30">
+      <c r="A9" s="17">
         <v>27</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="17">
         <v>7</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2"/>
@@ -2463,16 +2463,16 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="31">
+      <c r="A10" s="18">
         <v>19</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="19">
         <v>8.1</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="19" t="s">
         <v>4</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -2485,16 +2485,16 @@
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="30">
+      <c r="A11" s="17">
         <v>28</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="18">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="19" t="s">
         <v>4</v>
       </c>
       <c r="F11" s="2"/>
@@ -2505,16 +2505,16 @@
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="30">
+      <c r="A12" s="17">
         <v>21</v>
       </c>
-      <c r="B12" s="30">
+      <c r="B12" s="17">
         <v>6.7</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="2"/>
@@ -2525,16 +2525,16 @@
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="30">
+      <c r="A13" s="17">
         <v>22</v>
       </c>
-      <c r="B13" s="31">
+      <c r="B13" s="18">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="19" t="s">
         <v>4</v>
       </c>
       <c r="F13" s="2"/>
@@ -2543,16 +2543,16 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="30">
+      <c r="A14" s="17">
         <v>23</v>
       </c>
-      <c r="B14" s="30">
+      <c r="B14" s="17">
         <v>7.6</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F14" s="2"/>
@@ -2561,16 +2561,16 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="30">
+      <c r="A15" s="17">
         <v>25</v>
       </c>
-      <c r="B15" s="32">
+      <c r="B15" s="19">
         <v>9</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="19" t="s">
         <v>4</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -2583,16 +2583,16 @@
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="30">
+      <c r="A16" s="17">
         <v>27</v>
       </c>
-      <c r="B16" s="30">
+      <c r="B16" s="17">
         <v>7.4</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F16" s="2"/>
@@ -2603,16 +2603,16 @@
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="32">
+      <c r="A17" s="19">
         <v>30</v>
       </c>
-      <c r="B17" s="31">
+      <c r="B17" s="18">
         <v>4.9000000000000004</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="D17" s="19" t="s">
         <v>4</v>
       </c>
       <c r="F17" s="2"/>
@@ -2623,16 +2623,16 @@
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="32">
+      <c r="A18" s="19">
         <v>31</v>
       </c>
-      <c r="B18" s="31">
+      <c r="B18" s="18">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="19" t="s">
         <v>4</v>
       </c>
       <c r="F18" s="2"/>
@@ -2641,16 +2641,16 @@
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="32">
+      <c r="A19" s="19">
         <v>32</v>
       </c>
-      <c r="B19" s="30">
+      <c r="B19" s="17">
         <v>6.2</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="32" t="s">
+      <c r="D19" s="19" t="s">
         <v>4</v>
       </c>
       <c r="F19" s="2" t="s">
@@ -2663,16 +2663,16 @@
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="32">
+      <c r="A20" s="19">
         <v>33</v>
       </c>
-      <c r="B20" s="30">
+      <c r="B20" s="17">
         <v>7.5</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="19" t="s">
         <v>4</v>
       </c>
       <c r="F20" s="2"/>
@@ -2683,16 +2683,16 @@
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="30">
+      <c r="A21" s="17">
         <v>21</v>
       </c>
-      <c r="B21" s="31">
+      <c r="B21" s="18">
         <v>5.4</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="19" t="s">
         <v>4</v>
       </c>
       <c r="F21" s="2"/>
@@ -2703,58 +2703,58 @@
       <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="30">
+      <c r="A22" s="17">
         <v>22</v>
       </c>
-      <c r="B22" s="30">
+      <c r="B22" s="17">
         <v>6.7</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="17" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="30">
+      <c r="A23" s="17">
         <v>23</v>
       </c>
-      <c r="B23" s="30">
+      <c r="B23" s="17">
         <v>7.1</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="17" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="30">
+      <c r="A24" s="17">
         <v>25</v>
       </c>
-      <c r="B24" s="32">
+      <c r="B24" s="19">
         <v>8.5</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="32" t="s">
+      <c r="D24" s="19" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="30">
+      <c r="A25" s="17">
         <v>26</v>
       </c>
-      <c r="B25" s="31">
+      <c r="B25" s="18">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="32" t="s">
+      <c r="D25" s="19" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2797,10 +2797,10 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="16">
+      <c r="A28" s="23">
         <v>1</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="26" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="12" t="s">
@@ -2813,12 +2813,12 @@
         <v>0</v>
       </c>
       <c r="F28" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G28" s="4">
         <v>0</v>
       </c>
-      <c r="H28" s="19"/>
+      <c r="H28" s="27"/>
       <c r="J28">
         <v>24</v>
       </c>
@@ -2834,8 +2834,8 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="17"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="26"/>
       <c r="C29" s="12" t="s">
         <v>45</v>
       </c>
@@ -2852,11 +2852,11 @@
         <f>((-E29/D29)*IMLOG2(E29/D29)+(-F29/D29)*IMLOG2(F29/D29))</f>
         <v>0.99750254636911539</v>
       </c>
-      <c r="H29" s="19"/>
+      <c r="H29" s="27"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="17"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="26"/>
       <c r="C30" s="12" t="s">
         <v>46</v>
       </c>
@@ -2873,100 +2873,100 @@
         <f>((-E30/D30)*IMLOG2(E30/D30)+(-F30/D30)*IMLOG2(F30/D30))</f>
         <v>0.72192809488736165</v>
       </c>
-      <c r="H30" s="19"/>
+      <c r="H30" s="27"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
       <c r="H31" s="4">
         <f>(M28)-((D28/J28)*G28)-((D29/J28)*G29)-((D30/J28)*G30)</f>
         <v>0.12290276653816085</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="33" t="s">
+      <c r="A32" s="23"/>
+      <c r="B32" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="34">
+      <c r="D32" s="20">
         <v>9</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="20">
         <v>0</v>
       </c>
-      <c r="F32" s="34">
+      <c r="F32" s="20">
         <v>9</v>
       </c>
-      <c r="G32" s="35">
+      <c r="G32" s="21">
         <v>0</v>
       </c>
-      <c r="H32" s="36"/>
+      <c r="H32" s="25"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="34" t="s">
+      <c r="A33" s="23"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="34">
+      <c r="D33" s="20">
         <v>12</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="20">
         <v>10</v>
       </c>
-      <c r="F33" s="34">
+      <c r="F33" s="20">
         <v>2</v>
       </c>
-      <c r="G33" s="35">
+      <c r="G33" s="21">
         <f>((-E33/D33)*IMLOG2(E33/D33)+(-F33/D33)*IMLOG2(F33/D33))</f>
         <v>0.650022421648355</v>
       </c>
-      <c r="H33" s="36"/>
+      <c r="H33" s="25"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="34" t="s">
+      <c r="A34" s="23"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="34">
+      <c r="D34" s="20">
         <v>3</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="20">
         <v>0</v>
       </c>
-      <c r="F34" s="34">
+      <c r="F34" s="20">
         <v>3</v>
       </c>
-      <c r="G34" s="35">
+      <c r="G34" s="21">
         <v>0</v>
       </c>
-      <c r="H34" s="36"/>
+      <c r="H34" s="25"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="35">
+      <c r="A35" s="23"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="21">
         <f>(M28)-((D32/J28)*G32)-((D33/J28)*G33)-((D34/J28)*G34)</f>
         <v>0.65485754582697375</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
-      <c r="B36" s="17" t="s">
+      <c r="A36" s="23"/>
+      <c r="B36" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C36" s="12" t="s">
@@ -2985,11 +2985,11 @@
         <f>((-E36/D36)*IMLOG2(E36/D36)+(-F36/D36)*IMLOG2(F36/D36))</f>
         <v>0.99107605983822111</v>
       </c>
-      <c r="H36" s="19"/>
+      <c r="H36" s="27"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
-      <c r="B37" s="17"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="12" t="s">
         <v>50</v>
       </c>
@@ -3006,21 +3006,21 @@
         <f>((-E37/D37)*IMLOG2(E37/D37)+(-F37/D37)*IMLOG2(F37/D37))</f>
         <v>0.97095059445466747</v>
       </c>
-      <c r="H37" s="19"/>
+      <c r="H37" s="27"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
-      <c r="B38" s="17"/>
+      <c r="A38" s="23"/>
+      <c r="B38" s="26"/>
       <c r="C38" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D38" s="20">
+      <c r="D38" s="16">
         <v>0</v>
       </c>
-      <c r="E38" s="20">
+      <c r="E38" s="16">
         <v>0</v>
       </c>
-      <c r="F38" s="20">
+      <c r="F38" s="16">
         <v>0</v>
       </c>
       <c r="G38" s="4">
@@ -3029,13 +3029,13 @@
       <c r="H38" s="4"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
       <c r="H39" s="14">
         <f>(M28)-((D36/J28)*G36)-((D37/J28)*G37)-((D38/J28)*G38)</f>
         <v>1.3711126776512206E-3</v>
@@ -3093,28 +3093,28 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="16">
+      <c r="A42" s="23">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B42" s="33" t="s">
+      <c r="B42" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="34" t="s">
+      <c r="C42" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D42" s="34">
+      <c r="D42" s="20">
         <v>0</v>
       </c>
-      <c r="E42" s="34">
+      <c r="E42" s="20">
         <v>0</v>
       </c>
-      <c r="F42" s="34">
+      <c r="F42" s="20">
         <v>0</v>
       </c>
-      <c r="G42" s="35">
+      <c r="G42" s="21">
         <v>0</v>
       </c>
-      <c r="H42" s="36"/>
+      <c r="H42" s="25"/>
       <c r="J42">
         <v>12</v>
       </c>
@@ -3130,102 +3130,102 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
-      <c r="B43" s="33"/>
-      <c r="C43" s="34" t="s">
+      <c r="A43" s="23"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="34">
+      <c r="D43" s="20">
         <v>9</v>
       </c>
-      <c r="E43" s="34">
+      <c r="E43" s="20">
         <v>9</v>
       </c>
-      <c r="F43" s="34">
+      <c r="F43" s="20">
         <v>0</v>
       </c>
-      <c r="G43" s="35">
+      <c r="G43" s="21">
         <v>0</v>
       </c>
-      <c r="H43" s="36"/>
+      <c r="H43" s="25"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
-      <c r="B44" s="33"/>
-      <c r="C44" s="34" t="s">
+      <c r="A44" s="23"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D44" s="34">
+      <c r="D44" s="20">
         <v>3</v>
       </c>
-      <c r="E44" s="34">
+      <c r="E44" s="20">
         <v>1</v>
       </c>
-      <c r="F44" s="34">
+      <c r="F44" s="20">
         <v>2</v>
       </c>
-      <c r="G44" s="35">
+      <c r="G44" s="21">
         <f>((-E44/D44)*IMLOG2(E44/D44)+(-F44/D44)*IMLOG2(F44/D44))</f>
         <v>0.91829583405449056</v>
       </c>
-      <c r="H44" s="36"/>
+      <c r="H44" s="25"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
-      <c r="B45" s="33"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="35">
+      <c r="A45" s="23"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="21">
         <f>(M42)-((D42/J42)*G42)-((D43/J42)*G43)-((D44/J42)*G44)</f>
         <v>0.42044846313473239</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="23"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="31"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="26"/>
+      <c r="A47" s="23"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="34"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="16"/>
-      <c r="B48" s="24"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="26"/>
+      <c r="A48" s="23"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="34"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="28"/>
-      <c r="H49" s="29"/>
+      <c r="A49" s="23"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="37"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="16"/>
-      <c r="B50" s="17" t="s">
+      <c r="A50" s="23"/>
+      <c r="B50" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C50" s="12" t="s">
@@ -3243,11 +3243,11 @@
       <c r="G50" s="13">
         <v>0</v>
       </c>
-      <c r="H50" s="19"/>
+      <c r="H50" s="27"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="16"/>
-      <c r="B51" s="17"/>
+      <c r="A51" s="23"/>
+      <c r="B51" s="26"/>
       <c r="C51" s="12" t="s">
         <v>50</v>
       </c>
@@ -3264,21 +3264,21 @@
         <f>((-E51/D51)*IMLOG2(E51/D51)+(-F51/D51)*IMLOG2(F51/D51))</f>
         <v>0.81127812445913294</v>
       </c>
-      <c r="H51" s="19"/>
+      <c r="H51" s="27"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="16"/>
-      <c r="B52" s="17"/>
+      <c r="A52" s="23"/>
+      <c r="B52" s="26"/>
       <c r="C52" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="20">
+      <c r="D52" s="16">
         <v>0</v>
       </c>
-      <c r="E52" s="20">
+      <c r="E52" s="16">
         <v>0</v>
       </c>
-      <c r="F52" s="20">
+      <c r="F52" s="16">
         <v>0</v>
       </c>
       <c r="G52" s="13">
@@ -3287,13 +3287,13 @@
       <c r="H52" s="13"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
+      <c r="A53" s="23"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="28"/>
+      <c r="G53" s="28"/>
       <c r="H53" s="14">
         <f>(M42)-((D50/J42)*G50)-((D51/J42)*G51)-((D52/J42)*G52)</f>
         <v>0.10917033867559978</v>
@@ -3303,24 +3303,16 @@
       <c r="J55" s="2"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J56" s="37"/>
+      <c r="J56" s="22"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J57" s="37"/>
+      <c r="J57" s="22"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J58" s="37"/>
+      <c r="J58" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A42:A53"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="H42:H44"/>
-    <mergeCell ref="C45:G45"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="H50:H51"/>
-    <mergeCell ref="C53:G53"/>
-    <mergeCell ref="B46:H49"/>
     <mergeCell ref="A28:A39"/>
     <mergeCell ref="B36:B39"/>
     <mergeCell ref="C39:G39"/>
@@ -3331,6 +3323,14 @@
     <mergeCell ref="H32:H34"/>
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="H36:H37"/>
+    <mergeCell ref="A42:A53"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="H42:H44"/>
+    <mergeCell ref="C45:G45"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="C53:G53"/>
+    <mergeCell ref="B46:H49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>